<commit_message>
estructura de datos para parquimetros
</commit_message>
<xml_diff>
--- a/esquema de tablas.xlsx
+++ b/esquema de tablas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\spike-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86351960-B7A1-45B6-A69E-E0FFBEB92B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA42C73-59DA-45F0-8424-A87BEA89859B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4C5DF5BB-AA7F-4050-81B8-ADCB707D7105}"/>
+    <workbookView xWindow="38670" yWindow="420" windowWidth="28800" windowHeight="15345" xr2:uid="{4C5DF5BB-AA7F-4050-81B8-ADCB707D7105}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -169,11 +169,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BED51A9-9305-4FEF-B17F-BC8CC0D7BB0B}">
   <dimension ref="A2:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,207 +615,207 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="3">
-        <v>1</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="3">
-        <v>1</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>2</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>2</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>2</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>3</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="3">
-        <v>1</v>
-      </c>
-      <c r="O6" s="3" t="s">
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>4</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <v>3</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>5</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <v>4</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>